<commit_message>
Update to Forage Box V3
Removes full field map and biomass cut maps. Updates for On-farm beta test 2022.
</commit_message>
<xml_diff>
--- a/forms/psa_forage/psa_forage.xlsx
+++ b/forms/psa_forage/psa_forage.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saseehav\Documents\GitHub\Kobo\forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saseehav\Documents\GitHub\Kobo\forms\psa_forage\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
   <si>
     <t>type</t>
   </si>
@@ -56,27 +56,6 @@
     <t>list_name</t>
   </si>
   <si>
-    <t>map_c1</t>
-  </si>
-  <si>
-    <t>map_b1</t>
-  </si>
-  <si>
-    <t>map_c2</t>
-  </si>
-  <si>
-    <t>map_b2</t>
-  </si>
-  <si>
-    <t>map_c3</t>
-  </si>
-  <si>
-    <t>map_f1</t>
-  </si>
-  <si>
-    <t>map_c4</t>
-  </si>
-  <si>
     <t>today</t>
   </si>
   <si>
@@ -107,15 +86,6 @@
     <t>issues</t>
   </si>
   <si>
-    <t>IMAGE: Stand at the beginning of the strips, center yourself between the cover crop and bare strip, hold the tablet chest high, and take a photo of Rep 1</t>
-  </si>
-  <si>
-    <t>IMAGE: Stand at the beginning of the strips, center yourself between the cover crop and bare strip, hold the tablet chest high, and take a photo of Rep 2</t>
-  </si>
-  <si>
-    <t>note_with_walk_order</t>
-  </si>
-  <si>
     <t>form_name</t>
   </si>
   <si>
@@ -158,9 +128,6 @@
     <t>time</t>
   </si>
   <si>
-    <t>${time}='early'</t>
-  </si>
-  <si>
     <t>growth_stage_grains</t>
   </si>
   <si>
@@ -197,9 +164,6 @@
     <t>Ripening (grain forming from milk to kernel)</t>
   </si>
   <si>
-    <t>${time}='biomass'</t>
-  </si>
-  <si>
     <t>welcome</t>
   </si>
   <si>
@@ -218,62 +182,38 @@
     <t>No</t>
   </si>
   <si>
-    <t>select_one my95g71</t>
-  </si>
-  <si>
-    <t>field</t>
-  </si>
-  <si>
-    <t>Upload file from the Field walk (F1)</t>
-  </si>
-  <si>
-    <t>Upload forage box file Rep 1 Bare Ground Map (B1)</t>
-  </si>
-  <si>
-    <t>Upload forage box file Rep 1 Cover Crop Map (C1)</t>
-  </si>
-  <si>
-    <t>Upload forage box file Rep 2 Cover Crop Map (C2)</t>
-  </si>
-  <si>
-    <t>Upload forage box file Rep 2 Bare Ground Map (B2)</t>
-  </si>
-  <si>
-    <t>Upload file from biomass scan Rep 1 Cover Crop (C3)</t>
-  </si>
-  <si>
-    <t>Upload file from biomass scan Rep 2 Cover Crop (C4)</t>
-  </si>
-  <si>
-    <t>Is your field large enough (300' x 300' in addition to the strips) to do the field walk? And is their a buffer of 90' from obstructions like trees, ditches, and the trial?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Order of walks: Always start in the Bare strip first (for calibration), then do the 2 Cover Crop strips, followed by the 2nd Bare strip. </t>
-  </si>
-  <si>
     <t>psa_forage</t>
   </si>
   <si>
-    <t>ForageBoxWalkingPaths.jpg</t>
-  </si>
-  <si>
-    <t>Foragecloseup.jpg</t>
-  </si>
-  <si>
     <t>Do you have any issues to report? (including height of pole and movement of box)</t>
   </si>
   <si>
-    <t>v2</t>
-  </si>
-  <si>
-    <t>${field}='yes'</t>
+    <t>v3</t>
+  </si>
+  <si>
+    <t>Upload forage box file Map 1</t>
+  </si>
+  <si>
+    <t>Upload foage box file Map 2</t>
+  </si>
+  <si>
+    <t>map1</t>
+  </si>
+  <si>
+    <t>map2</t>
+  </si>
+  <si>
+    <t>Take a birds eye photo of the cover crop. Stand in the cover crop - Rep 1. hold the tablet chest high, point down. (be sure to remove your feet from the image)</t>
+  </si>
+  <si>
+    <t>Take a birds eye photo of the cover crop. Stand in the cover crop - Rep 2. hold the tablet chest high, point down. (be sure to remove your feet from the image)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,19 +221,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -308,9 +249,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -320,6 +260,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -625,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -638,9 +582,9 @@
     <col min="3" max="3" width="53.81640625" customWidth="1"/>
     <col min="4" max="4" width="6.6328125" customWidth="1"/>
     <col min="5" max="5" width="13.26953125" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="4"/>
-    <col min="7" max="7" width="16" style="2" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" style="2"/>
+    <col min="6" max="6" width="8.7265625" style="3"/>
+    <col min="7" max="7" width="16" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -654,19 +598,19 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -687,53 +631,53 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F7" s="5" t="s">
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -742,40 +686,40 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="4" t="b">
+        <v>15</v>
+      </c>
+      <c r="F9" s="3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="4" t="b">
+        <v>34</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="3" t="b">
         <v>0</v>
       </c>
     </row>
@@ -784,12 +728,12 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="4" t="b">
+        <v>16</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="3" t="b">
         <v>0</v>
       </c>
     </row>
@@ -798,186 +742,74 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="4" t="b">
+      <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="3" t="b">
         <v>0</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>66</v>
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
-      </c>
-      <c r="F14" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>78</v>
+        <v>59</v>
+      </c>
+      <c r="C15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" t="s">
-        <v>69</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" t="s">
-        <v>71</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" t="s">
-        <v>72</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" t="s">
-        <v>73</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" t="s">
-        <v>79</v>
-      </c>
-      <c r="F23" s="4" t="b">
+        <v>54</v>
+      </c>
+      <c r="F16" s="3" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1010,10 +842,10 @@
         <v>1234567</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1021,76 +853,76 @@
         <v>1234567</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>